<commit_message>
Add P16 and enable 2100 runs
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF41E84-68A5-498D-AFCC-1AF251D50AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A428EC-2C53-4B4B-9B89-355C50F60EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="59" r:id="rId1"/>
@@ -4043,21 +4043,21 @@
       <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.7265625" style="168" customWidth="1"/>
-    <col min="5" max="6" width="14.1796875" style="168" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" style="168" customWidth="1"/>
-    <col min="8" max="10" width="8.1796875" style="168" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" style="168" customWidth="1"/>
-    <col min="12" max="12" width="8.1796875" style="168" customWidth="1"/>
+    <col min="1" max="4" width="21.7109375" style="168" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" style="168" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="168" customWidth="1"/>
+    <col min="8" max="10" width="8.140625" style="168" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="168" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="168" customWidth="1"/>
     <col min="13" max="13" width="10" style="168" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="168" customWidth="1"/>
-    <col min="15" max="15" width="13.453125" style="168" customWidth="1"/>
-    <col min="16" max="16384" width="8.81640625" style="168"/>
+    <col min="14" max="14" width="11.42578125" style="168" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="168" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="168"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="166"/>
       <c r="B1" s="166"/>
       <c r="C1" s="166"/>
@@ -4085,7 +4085,7 @@
       <c r="Y1" s="167"/>
       <c r="Z1" s="167"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="166"/>
       <c r="B2" s="166"/>
       <c r="C2" s="166"/>
@@ -4113,7 +4113,7 @@
       <c r="Y2" s="167"/>
       <c r="Z2" s="167"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="166"/>
       <c r="B3" s="166"/>
       <c r="C3" s="166"/>
@@ -4141,7 +4141,7 @@
       <c r="Y3" s="167"/>
       <c r="Z3" s="167"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="166"/>
       <c r="B4" s="166"/>
       <c r="C4" s="166"/>
@@ -4169,7 +4169,7 @@
       <c r="Y4" s="167"/>
       <c r="Z4" s="167"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="166"/>
       <c r="B5" s="166"/>
       <c r="C5" s="166"/>
@@ -4197,7 +4197,7 @@
       <c r="Y5" s="167"/>
       <c r="Z5" s="167"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="166"/>
       <c r="B6" s="166"/>
       <c r="C6" s="166"/>
@@ -4225,7 +4225,7 @@
       <c r="Y6" s="167"/>
       <c r="Z6" s="167"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="166"/>
       <c r="B7" s="166"/>
       <c r="C7" s="166"/>
@@ -4253,7 +4253,7 @@
       <c r="Y7" s="167"/>
       <c r="Z7" s="167"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="166"/>
       <c r="B8" s="166"/>
       <c r="C8" s="166"/>
@@ -4281,7 +4281,7 @@
       <c r="Y8" s="167"/>
       <c r="Z8" s="167"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="166"/>
       <c r="B9" s="166"/>
       <c r="C9" s="166"/>
@@ -4309,7 +4309,7 @@
       <c r="Y9" s="167"/>
       <c r="Z9" s="167"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="166"/>
       <c r="B10" s="166"/>
       <c r="C10" s="166"/>
@@ -4337,7 +4337,7 @@
       <c r="Y10" s="167"/>
       <c r="Z10" s="167"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="166"/>
       <c r="B11" s="166"/>
       <c r="C11" s="166"/>
@@ -4365,7 +4365,7 @@
       <c r="Y11" s="167"/>
       <c r="Z11" s="167"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="166"/>
       <c r="B12" s="166"/>
       <c r="C12" s="166"/>
@@ -4393,7 +4393,7 @@
       <c r="Y12" s="167"/>
       <c r="Z12" s="167"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="166"/>
       <c r="B13" s="166"/>
       <c r="C13" s="166"/>
@@ -4421,7 +4421,7 @@
       <c r="Y13" s="167"/>
       <c r="Z13" s="167"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="166"/>
       <c r="B14" s="166"/>
       <c r="C14" s="166"/>
@@ -4449,7 +4449,7 @@
       <c r="Y14" s="167"/>
       <c r="Z14" s="167"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="166"/>
       <c r="B15" s="166"/>
       <c r="C15" s="166"/>
@@ -4477,7 +4477,7 @@
       <c r="Y15" s="167"/>
       <c r="Z15" s="167"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="203" t="s">
         <v>205</v>
       </c>
@@ -4507,7 +4507,7 @@
       <c r="Y16" s="167"/>
       <c r="Z16" s="167"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="171"/>
       <c r="B17" s="171"/>
       <c r="C17" s="171"/>
@@ -4535,7 +4535,7 @@
       <c r="Y17" s="167"/>
       <c r="Z17" s="167"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="171"/>
       <c r="B18" s="171"/>
       <c r="C18" s="171"/>
@@ -4563,7 +4563,7 @@
       <c r="Y18" s="167"/>
       <c r="Z18" s="167"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="174" t="s">
         <v>0</v>
       </c>
@@ -4595,7 +4595,7 @@
       <c r="Y19" s="167"/>
       <c r="Z19" s="167"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="174" t="s">
         <v>206</v>
       </c>
@@ -4627,7 +4627,7 @@
       <c r="Y20" s="167"/>
       <c r="Z20" s="167"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="174" t="s">
         <v>207</v>
       </c>
@@ -4659,7 +4659,7 @@
       <c r="Y21" s="167"/>
       <c r="Z21" s="167"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="174"/>
       <c r="B22" s="177"/>
       <c r="C22" s="177"/>
@@ -4687,7 +4687,7 @@
       <c r="Y22" s="167"/>
       <c r="Z22" s="167"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="174" t="s">
         <v>208</v>
       </c>
@@ -4719,7 +4719,7 @@
       <c r="Y23" s="167"/>
       <c r="Z23" s="167"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="174"/>
       <c r="B24" s="202" t="s">
         <v>219</v>
@@ -4749,7 +4749,7 @@
       <c r="Y24" s="167"/>
       <c r="Z24" s="167"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="174"/>
       <c r="B25" s="177"/>
       <c r="C25" s="177"/>
@@ -4777,7 +4777,7 @@
       <c r="Y25" s="167"/>
       <c r="Z25" s="167"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="174" t="s">
         <v>209</v>
       </c>
@@ -4809,7 +4809,7 @@
       <c r="Y26" s="167"/>
       <c r="Z26" s="167"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="174"/>
       <c r="B27" s="202" t="s">
         <v>220</v>
@@ -4839,7 +4839,7 @@
       <c r="Y27" s="167"/>
       <c r="Z27" s="167"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="174"/>
       <c r="B28" s="177"/>
       <c r="C28" s="177"/>
@@ -4867,7 +4867,7 @@
       <c r="Y28" s="167"/>
       <c r="Z28" s="167"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="174" t="s">
         <v>210</v>
       </c>
@@ -4899,7 +4899,7 @@
       <c r="Y29" s="167"/>
       <c r="Z29" s="167"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="174" t="s">
         <v>211</v>
       </c>
@@ -4931,7 +4931,7 @@
       <c r="Y30" s="167"/>
       <c r="Z30" s="167"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="174" t="s">
         <v>213</v>
       </c>
@@ -4963,7 +4963,7 @@
       <c r="Y31" s="167"/>
       <c r="Z31" s="167"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="180"/>
       <c r="B32" s="181" t="s">
         <v>215</v>
@@ -4993,7 +4993,7 @@
       <c r="Y32" s="167"/>
       <c r="Z32" s="167"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="166"/>
       <c r="B33" s="166"/>
       <c r="C33" s="166"/>
@@ -5021,7 +5021,7 @@
       <c r="Y33" s="167"/>
       <c r="Z33" s="167"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="166"/>
       <c r="B34" s="166"/>
       <c r="C34" s="166"/>
@@ -5049,7 +5049,7 @@
       <c r="Y34" s="167"/>
       <c r="Z34" s="167"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="166"/>
       <c r="B35" s="166"/>
       <c r="C35" s="166"/>
@@ -5077,7 +5077,7 @@
       <c r="Y35" s="167"/>
       <c r="Z35" s="167"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="166"/>
       <c r="B36" s="166"/>
       <c r="C36" s="166"/>
@@ -5105,7 +5105,7 @@
       <c r="Y36" s="167"/>
       <c r="Z36" s="167"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="166"/>
       <c r="B37" s="166"/>
       <c r="C37" s="166"/>
@@ -5133,7 +5133,7 @@
       <c r="Y37" s="167"/>
       <c r="Z37" s="167"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="166"/>
       <c r="B38" s="166"/>
       <c r="C38" s="166"/>
@@ -5161,7 +5161,7 @@
       <c r="Y38" s="167"/>
       <c r="Z38" s="167"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="166"/>
       <c r="B39" s="166"/>
       <c r="C39" s="166"/>
@@ -5189,7 +5189,7 @@
       <c r="Y39" s="167"/>
       <c r="Z39" s="167"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="166"/>
       <c r="B40" s="166"/>
       <c r="C40" s="166"/>
@@ -5217,7 +5217,7 @@
       <c r="Y40" s="167"/>
       <c r="Z40" s="167"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="166"/>
       <c r="B41" s="166"/>
       <c r="C41" s="166"/>
@@ -5245,7 +5245,7 @@
       <c r="Y41" s="167"/>
       <c r="Z41" s="167"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="166"/>
       <c r="B42" s="166"/>
       <c r="C42" s="166"/>
@@ -5273,7 +5273,7 @@
       <c r="Y42" s="167"/>
       <c r="Z42" s="167"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="167"/>
       <c r="B43" s="167"/>
       <c r="C43" s="167"/>
@@ -5301,7 +5301,7 @@
       <c r="Y43" s="167"/>
       <c r="Z43" s="167"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="167"/>
       <c r="B44" s="167"/>
       <c r="C44" s="167"/>
@@ -5329,7 +5329,7 @@
       <c r="Y44" s="167"/>
       <c r="Z44" s="167"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="167"/>
       <c r="B45" s="167"/>
       <c r="C45" s="167"/>
@@ -5357,7 +5357,7 @@
       <c r="Y45" s="167"/>
       <c r="Z45" s="167"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="167"/>
       <c r="B46" s="167"/>
       <c r="C46" s="167"/>
@@ -5385,7 +5385,7 @@
       <c r="Y46" s="167"/>
       <c r="Z46" s="167"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="167"/>
       <c r="B47" s="167"/>
       <c r="C47" s="167"/>
@@ -5413,7 +5413,7 @@
       <c r="Y47" s="167"/>
       <c r="Z47" s="167"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="167"/>
       <c r="B48" s="167"/>
       <c r="C48" s="167"/>
@@ -5441,7 +5441,7 @@
       <c r="Y48" s="167"/>
       <c r="Z48" s="167"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="167"/>
       <c r="B49" s="167"/>
       <c r="C49" s="167"/>
@@ -5469,7 +5469,7 @@
       <c r="Y49" s="167"/>
       <c r="Z49" s="167"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="167"/>
       <c r="B50" s="167"/>
       <c r="C50" s="167"/>
@@ -5497,7 +5497,7 @@
       <c r="Y50" s="167"/>
       <c r="Z50" s="167"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="167"/>
       <c r="B51" s="167"/>
       <c r="C51" s="167"/>
@@ -5525,7 +5525,7 @@
       <c r="Y51" s="167"/>
       <c r="Z51" s="167"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="167"/>
       <c r="B52" s="167"/>
       <c r="C52" s="167"/>
@@ -5553,7 +5553,7 @@
       <c r="Y52" s="167"/>
       <c r="Z52" s="167"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="167"/>
       <c r="B53" s="167"/>
       <c r="C53" s="167"/>
@@ -5581,7 +5581,7 @@
       <c r="Y53" s="167"/>
       <c r="Z53" s="167"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="167"/>
       <c r="B54" s="167"/>
       <c r="C54" s="167"/>
@@ -5609,7 +5609,7 @@
       <c r="Y54" s="167"/>
       <c r="Z54" s="167"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="167"/>
       <c r="B55" s="167"/>
       <c r="C55" s="167"/>
@@ -5637,7 +5637,7 @@
       <c r="Y55" s="167"/>
       <c r="Z55" s="167"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="167"/>
       <c r="B56" s="167"/>
       <c r="C56" s="167"/>
@@ -5665,7 +5665,7 @@
       <c r="Y56" s="167"/>
       <c r="Z56" s="167"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="167"/>
       <c r="B57" s="167"/>
       <c r="C57" s="167"/>
@@ -5693,7 +5693,7 @@
       <c r="Y57" s="167"/>
       <c r="Z57" s="167"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="167"/>
       <c r="B58" s="167"/>
       <c r="C58" s="167"/>
@@ -5721,7 +5721,7 @@
       <c r="Y58" s="167"/>
       <c r="Z58" s="167"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="167"/>
       <c r="B59" s="167"/>
       <c r="C59" s="167"/>
@@ -5749,7 +5749,7 @@
       <c r="Y59" s="167"/>
       <c r="Z59" s="167"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="167"/>
       <c r="B60" s="167"/>
       <c r="C60" s="167"/>
@@ -5777,7 +5777,7 @@
       <c r="Y60" s="167"/>
       <c r="Z60" s="167"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="167"/>
       <c r="B61" s="167"/>
       <c r="C61" s="167"/>
@@ -5805,7 +5805,7 @@
       <c r="Y61" s="167"/>
       <c r="Z61" s="167"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="167"/>
       <c r="B62" s="167"/>
       <c r="C62" s="167"/>
@@ -5833,7 +5833,7 @@
       <c r="Y62" s="167"/>
       <c r="Z62" s="167"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="167"/>
       <c r="B63" s="167"/>
       <c r="C63" s="167"/>
@@ -5861,7 +5861,7 @@
       <c r="Y63" s="167"/>
       <c r="Z63" s="167"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="167"/>
       <c r="B64" s="167"/>
       <c r="C64" s="167"/>
@@ -5889,7 +5889,7 @@
       <c r="Y64" s="167"/>
       <c r="Z64" s="167"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="167"/>
       <c r="B65" s="167"/>
       <c r="C65" s="167"/>
@@ -5917,7 +5917,7 @@
       <c r="Y65" s="167"/>
       <c r="Z65" s="167"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="167"/>
       <c r="B66" s="167"/>
       <c r="C66" s="167"/>
@@ -5945,7 +5945,7 @@
       <c r="Y66" s="167"/>
       <c r="Z66" s="167"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="167"/>
       <c r="B67" s="167"/>
       <c r="C67" s="167"/>
@@ -5973,7 +5973,7 @@
       <c r="Y67" s="167"/>
       <c r="Z67" s="167"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="167"/>
       <c r="B68" s="167"/>
       <c r="C68" s="167"/>
@@ -6001,7 +6001,7 @@
       <c r="Y68" s="167"/>
       <c r="Z68" s="167"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="167"/>
       <c r="B69" s="167"/>
       <c r="C69" s="167"/>
@@ -6029,7 +6029,7 @@
       <c r="Y69" s="167"/>
       <c r="Z69" s="167"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="167"/>
       <c r="B70" s="167"/>
       <c r="C70" s="167"/>
@@ -6057,7 +6057,7 @@
       <c r="Y70" s="167"/>
       <c r="Z70" s="167"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="167"/>
       <c r="B71" s="167"/>
       <c r="C71" s="167"/>
@@ -6085,7 +6085,7 @@
       <c r="Y71" s="167"/>
       <c r="Z71" s="167"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="167"/>
       <c r="B72" s="167"/>
       <c r="C72" s="167"/>
@@ -6113,7 +6113,7 @@
       <c r="Y72" s="167"/>
       <c r="Z72" s="167"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="167"/>
       <c r="B73" s="167"/>
       <c r="C73" s="167"/>
@@ -6141,7 +6141,7 @@
       <c r="Y73" s="167"/>
       <c r="Z73" s="167"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="167"/>
       <c r="B74" s="167"/>
       <c r="C74" s="167"/>
@@ -6169,7 +6169,7 @@
       <c r="Y74" s="167"/>
       <c r="Z74" s="167"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="167"/>
       <c r="B75" s="167"/>
       <c r="C75" s="167"/>
@@ -6197,7 +6197,7 @@
       <c r="Y75" s="167"/>
       <c r="Z75" s="167"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="167"/>
       <c r="B76" s="167"/>
       <c r="C76" s="167"/>
@@ -6225,7 +6225,7 @@
       <c r="Y76" s="167"/>
       <c r="Z76" s="167"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="167"/>
       <c r="B77" s="167"/>
       <c r="C77" s="167"/>
@@ -6253,7 +6253,7 @@
       <c r="Y77" s="167"/>
       <c r="Z77" s="167"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="167"/>
       <c r="B78" s="167"/>
       <c r="C78" s="167"/>
@@ -6281,7 +6281,7 @@
       <c r="Y78" s="167"/>
       <c r="Z78" s="167"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="167"/>
       <c r="B79" s="167"/>
       <c r="C79" s="167"/>
@@ -6309,7 +6309,7 @@
       <c r="Y79" s="167"/>
       <c r="Z79" s="167"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="167"/>
       <c r="B80" s="167"/>
       <c r="C80" s="167"/>
@@ -6337,7 +6337,7 @@
       <c r="Y80" s="167"/>
       <c r="Z80" s="167"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="167"/>
       <c r="B81" s="167"/>
       <c r="C81" s="167"/>
@@ -6365,7 +6365,7 @@
       <c r="Y81" s="167"/>
       <c r="Z81" s="167"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="167"/>
       <c r="B82" s="167"/>
       <c r="C82" s="167"/>
@@ -6393,7 +6393,7 @@
       <c r="Y82" s="167"/>
       <c r="Z82" s="167"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="167"/>
       <c r="B83" s="167"/>
       <c r="C83" s="167"/>
@@ -6421,7 +6421,7 @@
       <c r="Y83" s="167"/>
       <c r="Z83" s="167"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="167"/>
       <c r="B84" s="167"/>
       <c r="C84" s="167"/>
@@ -6449,7 +6449,7 @@
       <c r="Y84" s="167"/>
       <c r="Z84" s="167"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="167"/>
       <c r="B85" s="167"/>
       <c r="C85" s="167"/>
@@ -6477,7 +6477,7 @@
       <c r="Y85" s="167"/>
       <c r="Z85" s="167"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="167"/>
       <c r="B86" s="167"/>
       <c r="C86" s="167"/>
@@ -6505,7 +6505,7 @@
       <c r="Y86" s="167"/>
       <c r="Z86" s="167"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="167"/>
       <c r="B87" s="167"/>
       <c r="C87" s="167"/>
@@ -6533,7 +6533,7 @@
       <c r="Y87" s="167"/>
       <c r="Z87" s="167"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="167"/>
       <c r="B88" s="167"/>
       <c r="C88" s="167"/>
@@ -6561,7 +6561,7 @@
       <c r="Y88" s="167"/>
       <c r="Z88" s="167"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="167"/>
       <c r="B89" s="167"/>
       <c r="C89" s="167"/>
@@ -6589,7 +6589,7 @@
       <c r="Y89" s="167"/>
       <c r="Z89" s="167"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="167"/>
       <c r="B90" s="167"/>
       <c r="C90" s="167"/>
@@ -6617,7 +6617,7 @@
       <c r="Y90" s="167"/>
       <c r="Z90" s="167"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="167"/>
       <c r="B91" s="167"/>
       <c r="C91" s="167"/>
@@ -6645,7 +6645,7 @@
       <c r="Y91" s="167"/>
       <c r="Z91" s="167"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="167"/>
       <c r="B92" s="167"/>
       <c r="C92" s="167"/>
@@ -6673,7 +6673,7 @@
       <c r="Y92" s="167"/>
       <c r="Z92" s="167"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="167"/>
       <c r="B93" s="167"/>
       <c r="C93" s="167"/>
@@ -6701,7 +6701,7 @@
       <c r="Y93" s="167"/>
       <c r="Z93" s="167"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="167"/>
       <c r="B94" s="167"/>
       <c r="C94" s="167"/>
@@ -6729,7 +6729,7 @@
       <c r="Y94" s="167"/>
       <c r="Z94" s="167"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="167"/>
       <c r="B95" s="167"/>
       <c r="C95" s="167"/>
@@ -6757,7 +6757,7 @@
       <c r="Y95" s="167"/>
       <c r="Z95" s="167"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="167"/>
       <c r="B96" s="167"/>
       <c r="C96" s="167"/>
@@ -6785,7 +6785,7 @@
       <c r="Y96" s="167"/>
       <c r="Z96" s="167"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="167"/>
       <c r="B97" s="167"/>
       <c r="C97" s="167"/>
@@ -6813,7 +6813,7 @@
       <c r="Y97" s="167"/>
       <c r="Z97" s="167"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="167"/>
       <c r="B98" s="167"/>
       <c r="C98" s="167"/>
@@ -6841,7 +6841,7 @@
       <c r="Y98" s="167"/>
       <c r="Z98" s="167"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="167"/>
       <c r="B99" s="167"/>
       <c r="C99" s="167"/>
@@ -6902,21 +6902,21 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="93.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" style="3" customWidth="1"/>
-    <col min="5" max="6" width="11.453125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="3"/>
-    <col min="8" max="8" width="18.54296875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="96.54296875" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="3.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="93.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="18.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="96.5703125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="205" t="s">
         <v>1</v>
       </c>
@@ -6941,7 +6941,7 @@
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="2:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
@@ -6972,7 +6972,7 @@
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>69</v>
       </c>
@@ -7002,7 +7002,7 @@
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
@@ -7032,7 +7032,7 @@
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="17" t="s">
         <v>73</v>
       </c>
@@ -7064,7 +7064,7 @@
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>75</v>
       </c>
@@ -7094,7 +7094,7 @@
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>35</v>
       </c>
@@ -7124,7 +7124,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="2:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>79</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
         <v>81</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
         <v>82</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="s">
         <v>83</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>84</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="2:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>86</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>41</v>
       </c>
@@ -7230,7 +7230,7 @@
       </c>
       <c r="I15" s="207"/>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>8</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>9</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
         <v>10</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H19" s="44" t="s">
         <v>48</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="208" t="s">
         <v>49</v>
       </c>
@@ -7307,7 +7307,7 @@
       <c r="E20" s="210"/>
       <c r="F20" s="126"/>
     </row>
-    <row r="21" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="s">
         <v>30</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="38" t="s">
         <v>188</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="38" t="s">
         <v>193</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="131" t="s">
         <v>194</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="38" t="s">
         <v>195</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
         <v>51</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="131" t="s">
         <v>199</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
         <v>89</v>
       </c>
@@ -7449,9 +7449,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="205" t="s">
         <v>53</v>
       </c>
@@ -7464,7 +7464,7 @@
       </c>
       <c r="I38" s="212"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="49" t="s">
         <v>54</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" s="52" t="s">
         <v>16</v>
       </c>
@@ -7502,7 +7502,7 @@
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="52"/>
       <c r="C41" s="42"/>
       <c r="D41" s="42"/>
@@ -7511,14 +7511,14 @@
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="55"/>
       <c r="E42" s="56"/>
       <c r="F42" s="56"/>
       <c r="H42" s="42"/>
       <c r="I42" s="42"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" s="55"/>
       <c r="C43" s="57"/>
       <c r="D43" s="57"/>
@@ -7527,7 +7527,7 @@
       <c r="H43" s="42"/>
       <c r="I43" s="42"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="55"/>
       <c r="C44" s="57"/>
       <c r="D44" s="57"/>
@@ -7536,7 +7536,7 @@
       <c r="H44" s="42"/>
       <c r="I44" s="42"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H45" s="42"/>
       <c r="I45" s="42"/>
     </row>
@@ -7568,41 +7568,41 @@
   </sheetPr>
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="66" customWidth="1"/>
     <col min="2" max="2" width="18" style="66" customWidth="1"/>
-    <col min="3" max="3" width="33.453125" style="66" customWidth="1"/>
-    <col min="4" max="6" width="10.7265625" style="66" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="66" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" style="66" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="66" customWidth="1"/>
+    <col min="4" max="6" width="10.7109375" style="66" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="66" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="66" customWidth="1"/>
     <col min="9" max="9" width="2" style="66" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.453125" style="66" customWidth="1"/>
-    <col min="11" max="11" width="18.81640625" style="66" customWidth="1"/>
-    <col min="12" max="12" width="6.453125" style="66" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.1796875" style="66"/>
-    <col min="15" max="15" width="9.54296875" style="66" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" style="66"/>
-    <col min="17" max="21" width="11.1796875" style="66" customWidth="1"/>
-    <col min="22" max="16384" width="9.1796875" style="66"/>
+    <col min="10" max="10" width="22.42578125" style="66" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" style="66" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" style="66" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="66"/>
+    <col min="15" max="15" width="9.5703125" style="66" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="66"/>
+    <col min="17" max="21" width="11.140625" style="66" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="60" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="61"/>
     </row>
-    <row r="2" spans="1:21" ht="18.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A2" s="62" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
         <v>18</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -7675,7 +7675,7 @@
       </c>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="39.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
         <v>57</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="63" t="s">
         <v>27</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>RSDSH_Apt-AB</v>
       </c>
       <c r="L7" s="198">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M7" s="198">
         <v>50</v>
@@ -7792,7 +7792,7 @@
         <v>5.7348345211809249E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="68" t="s">
         <v>27</v>
       </c>
@@ -7823,7 +7823,7 @@
         <v>RSDSH_Apt-C</v>
       </c>
       <c r="L8" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M8" s="63">
         <v>50</v>
@@ -7855,7 +7855,7 @@
         <v>6.6924201054815937E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="63" t="s">
         <v>27</v>
       </c>
@@ -7886,7 +7886,7 @@
         <v>RSDSH_Apt-D</v>
       </c>
       <c r="L9" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M9" s="63">
         <v>50</v>
@@ -7918,7 +7918,7 @@
         <v>4.7948563185053724E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="68" t="s">
         <v>27</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>RSDSH_Apt-E</v>
       </c>
       <c r="L10" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M10" s="63">
         <v>50</v>
@@ -7981,7 +7981,7 @@
         <v>9.2808418616751667E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="63" t="s">
         <v>27</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>RSDSH_Apt-F</v>
       </c>
       <c r="L11" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M11" s="63">
         <v>50</v>
@@ -8044,7 +8044,7 @@
         <v>1.4628662883294537E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="68" t="s">
         <v>27</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>RSDSH_Apt-G</v>
       </c>
       <c r="L12" s="191">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M12" s="191">
         <v>50</v>
@@ -8107,7 +8107,7 @@
         <v>2.1717043475893594E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="63" t="s">
         <v>27</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>RSDSH_Att-AB</v>
       </c>
       <c r="L13" s="198">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M13" s="198">
         <v>50</v>
@@ -8170,7 +8170,7 @@
         <v>7.5821699232505875E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="68" t="s">
         <v>27</v>
       </c>
@@ -8201,7 +8201,7 @@
         <v>RSDSH_Att-C</v>
       </c>
       <c r="L14" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M14" s="63">
         <v>50</v>
@@ -8233,7 +8233,7 @@
         <v>8.8482180697850338E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="63" t="s">
         <v>27</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>RSDSH_Att-D</v>
       </c>
       <c r="L15" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M15" s="63">
         <v>50</v>
@@ -8296,7 +8296,7 @@
         <v>5.1655487686243003E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="68" t="s">
         <v>27</v>
       </c>
@@ -8327,7 +8327,7 @@
         <v>RSDSH_Att-E</v>
       </c>
       <c r="L16" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M16" s="63">
         <v>50</v>
@@ -8359,7 +8359,7 @@
         <v>9.3929668522173305E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="63" t="s">
         <v>27</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>RSDSH_Att-F</v>
       </c>
       <c r="L17" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M17" s="63">
         <v>50</v>
@@ -8422,7 +8422,7 @@
         <v>1.4727434391205585E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="68" t="s">
         <v>27</v>
       </c>
@@ -8453,7 +8453,7 @@
         <v>RSDSH_Att-G</v>
       </c>
       <c r="L18" s="191">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M18" s="191">
         <v>50</v>
@@ -8485,7 +8485,7 @@
         <v>2.1290335851398529E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="63" t="s">
         <v>27</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>RSDSH_Det-AB</v>
       </c>
       <c r="L19" s="198">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M19" s="198">
         <v>50</v>
@@ -8548,7 +8548,7 @@
         <v>8.7124448896018676E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="68" t="s">
         <v>27</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>RSDSH_Det-C</v>
       </c>
       <c r="L20" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M20" s="63">
         <v>50</v>
@@ -8611,7 +8611,7 @@
         <v>1.0167222982933634E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="63" t="s">
         <v>27</v>
       </c>
@@ -8642,7 +8642,7 @@
         <v>RSDSH_Det-D</v>
       </c>
       <c r="L21" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M21" s="63">
         <v>50</v>
@@ -8674,7 +8674,7 @@
         <v>5.2660659296241401E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="68" t="s">
         <v>27</v>
       </c>
@@ -8705,7 +8705,7 @@
         <v>RSDSH_Det-E</v>
       </c>
       <c r="L22" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M22" s="63">
         <v>50</v>
@@ -8737,7 +8737,7 @@
         <v>9.4356152934719911E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="63" t="s">
         <v>27</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>RSDSH_Det-F</v>
       </c>
       <c r="L23" s="63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M23" s="63">
         <v>50</v>
@@ -8800,7 +8800,7 @@
         <v>1.4628662883294537E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="68" t="s">
         <v>27</v>
       </c>
@@ -8831,7 +8831,7 @@
         <v>RSDSH_Det-G</v>
       </c>
       <c r="L24" s="191">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="M24" s="191">
         <v>50</v>
@@ -8863,224 +8863,224 @@
         <v>2.1717043475893594E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="V27"/>
       <c r="W27"/>
       <c r="X27"/>
       <c r="Y27"/>
       <c r="Z27"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="V28"/>
       <c r="W28"/>
       <c r="X28"/>
       <c r="Y28"/>
       <c r="Z28"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="V29"/>
       <c r="W29"/>
       <c r="X29"/>
       <c r="Y29"/>
       <c r="Z29"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="V30"/>
       <c r="W30"/>
       <c r="X30"/>
       <c r="Y30"/>
       <c r="Z30"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="V31"/>
       <c r="W31"/>
       <c r="X31"/>
       <c r="Y31"/>
       <c r="Z31"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="V32"/>
       <c r="W32"/>
       <c r="X32"/>
       <c r="Y32"/>
       <c r="Z32"/>
     </row>
-    <row r="33" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V33"/>
       <c r="W33"/>
       <c r="X33"/>
       <c r="Y33"/>
       <c r="Z33"/>
     </row>
-    <row r="34" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V34"/>
       <c r="W34"/>
       <c r="X34"/>
       <c r="Y34"/>
       <c r="Z34"/>
     </row>
-    <row r="35" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V35"/>
       <c r="W35"/>
       <c r="X35"/>
       <c r="Y35"/>
       <c r="Z35"/>
     </row>
-    <row r="36" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V36"/>
       <c r="W36"/>
       <c r="X36"/>
       <c r="Y36"/>
       <c r="Z36"/>
     </row>
-    <row r="37" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V37"/>
       <c r="W37"/>
       <c r="X37"/>
       <c r="Y37"/>
       <c r="Z37"/>
     </row>
-    <row r="38" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V38"/>
       <c r="W38"/>
       <c r="X38"/>
       <c r="Y38"/>
       <c r="Z38"/>
     </row>
-    <row r="39" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V39"/>
       <c r="W39"/>
       <c r="X39"/>
       <c r="Y39"/>
       <c r="Z39"/>
     </row>
-    <row r="40" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V40"/>
       <c r="W40"/>
       <c r="X40"/>
       <c r="Y40"/>
       <c r="Z40"/>
     </row>
-    <row r="41" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V41"/>
       <c r="W41"/>
       <c r="X41"/>
       <c r="Y41"/>
       <c r="Z41"/>
     </row>
-    <row r="42" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V42"/>
       <c r="W42"/>
       <c r="X42"/>
       <c r="Y42"/>
       <c r="Z42"/>
     </row>
-    <row r="43" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V43"/>
       <c r="W43"/>
       <c r="X43"/>
       <c r="Y43"/>
       <c r="Z43"/>
     </row>
-    <row r="44" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V44"/>
       <c r="W44"/>
       <c r="X44"/>
       <c r="Y44"/>
       <c r="Z44"/>
     </row>
-    <row r="45" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V45"/>
       <c r="W45"/>
       <c r="X45"/>
       <c r="Y45"/>
       <c r="Z45"/>
     </row>
-    <row r="46" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V46"/>
       <c r="W46"/>
       <c r="X46"/>
       <c r="Y46"/>
       <c r="Z46"/>
     </row>
-    <row r="47" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V47"/>
       <c r="W47"/>
       <c r="X47"/>
       <c r="Y47"/>
       <c r="Z47"/>
     </row>
-    <row r="48" spans="22:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="22:26" x14ac:dyDescent="0.2">
       <c r="V48"/>
       <c r="W48"/>
       <c r="X48"/>
       <c r="Y48"/>
       <c r="Z48"/>
     </row>
-    <row r="49" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V49"/>
       <c r="W49"/>
       <c r="X49"/>
       <c r="Y49"/>
       <c r="Z49"/>
     </row>
-    <row r="50" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V50"/>
       <c r="W50"/>
       <c r="X50"/>
       <c r="Y50"/>
       <c r="Z50"/>
     </row>
-    <row r="51" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V51"/>
       <c r="W51"/>
       <c r="X51"/>
       <c r="Y51"/>
       <c r="Z51"/>
     </row>
-    <row r="52" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V52"/>
       <c r="W52"/>
       <c r="X52"/>
       <c r="Y52"/>
       <c r="Z52"/>
     </row>
-    <row r="53" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V53"/>
       <c r="W53"/>
       <c r="X53"/>
       <c r="Y53"/>
       <c r="Z53"/>
     </row>
-    <row r="54" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V54"/>
       <c r="W54"/>
       <c r="X54"/>
       <c r="Y54"/>
       <c r="Z54"/>
     </row>
-    <row r="55" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V55"/>
       <c r="W55"/>
       <c r="X55"/>
       <c r="Y55"/>
       <c r="Z55"/>
     </row>
-    <row r="56" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V56"/>
       <c r="W56"/>
       <c r="X56"/>
       <c r="Y56"/>
       <c r="Z56"/>
     </row>
-    <row r="57" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="18:26" x14ac:dyDescent="0.2">
       <c r="V57"/>
       <c r="W57"/>
       <c r="X57"/>
       <c r="Y57"/>
       <c r="Z57"/>
     </row>
-    <row r="58" spans="18:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="18:26" x14ac:dyDescent="0.2">
       <c r="R58"/>
       <c r="U58"/>
       <c r="V58"/>
@@ -9106,33 +9106,33 @@
       <selection activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" customWidth="1"/>
-    <col min="13" max="13" width="13.1796875" customWidth="1"/>
-    <col min="14" max="15" width="13.54296875" customWidth="1"/>
-    <col min="16" max="18" width="10.7265625" customWidth="1"/>
-    <col min="19" max="19" width="12.453125" customWidth="1"/>
-    <col min="20" max="21" width="12.26953125" customWidth="1"/>
-    <col min="24" max="24" width="11.81640625" customWidth="1"/>
-    <col min="40" max="40" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="15" width="13.5703125" customWidth="1"/>
+    <col min="16" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="21" width="12.28515625" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" customWidth="1"/>
+    <col min="40" max="40" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:42" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L2" s="216" t="s">
         <v>167</v>
       </c>
@@ -9152,7 +9152,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="3:42" ht="21.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:42" ht="21.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="215" t="s">
         <v>156</v>
       </c>
@@ -9222,7 +9222,7 @@
       <c r="AO3" s="150"/>
       <c r="AP3" s="150"/>
     </row>
-    <row r="4" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="73" t="s">
         <v>160</v>
       </c>
@@ -9291,7 +9291,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="75" t="s">
         <v>111</v>
       </c>
@@ -9390,7 +9390,7 @@
         <v>1.3478893740902476</v>
       </c>
     </row>
-    <row r="6" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="80" t="s">
         <v>114</v>
       </c>
@@ -9489,7 +9489,7 @@
         <v>1.3478893740902476</v>
       </c>
     </row>
-    <row r="7" spans="3:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C7" s="85" t="s">
         <v>115</v>
       </c>
@@ -9588,7 +9588,7 @@
         <v>1.3478893740902476</v>
       </c>
     </row>
-    <row r="8" spans="3:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C8" s="80" t="s">
         <v>116</v>
       </c>
@@ -9687,7 +9687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:42" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:42" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="85" t="s">
         <v>118</v>
       </c>
@@ -9789,7 +9789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C10" s="80" t="s">
         <v>122</v>
       </c>
@@ -9888,7 +9888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C11" s="85" t="s">
         <v>125</v>
       </c>
@@ -9987,7 +9987,7 @@
         <v>0.65110565110565111</v>
       </c>
     </row>
-    <row r="12" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="80" t="s">
         <v>127</v>
       </c>
@@ -10084,7 +10084,7 @@
         <v>0.65110565110565111</v>
       </c>
     </row>
-    <row r="13" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="95" t="s">
         <v>128</v>
       </c>
@@ -10148,7 +10148,7 @@
         <v>0.65110565110565111</v>
       </c>
     </row>
-    <row r="14" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14" s="98" t="s">
         <v>163</v>
       </c>
@@ -10208,7 +10208,7 @@
         <v>0.67542972699696668</v>
       </c>
     </row>
-    <row r="15" spans="3:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:42" ht="15" x14ac:dyDescent="0.2">
       <c r="L15" t="s">
         <v>177</v>
       </c>
@@ -10251,7 +10251,7 @@
         <v>0.67542972699696668</v>
       </c>
     </row>
-    <row r="16" spans="3:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L16" s="2" t="s">
         <v>180</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>0.68787878787878787</v>
       </c>
     </row>
-    <row r="17" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F17" s="72" t="s">
         <v>158</v>
       </c>
@@ -10378,7 +10378,7 @@
         <v>0.68787878787878787</v>
       </c>
     </row>
-    <row r="18" spans="1:42" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>185</v>
       </c>
@@ -10476,7 +10476,7 @@
         <v>0.69895091794679653</v>
       </c>
     </row>
-    <row r="19" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>186</v>
       </c>
@@ -10565,7 +10565,7 @@
         <v>0.55669942286694751</v>
       </c>
     </row>
-    <row r="20" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>187</v>
       </c>
@@ -10614,7 +10614,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F21" s="108">
         <f>SUM(F18:F20)</f>
         <v>766351.7209999999</v>
@@ -10650,7 +10650,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="F22" s="72" t="s">
         <v>158</v>
       </c>
@@ -10684,7 +10684,7 @@
       <c r="V22" s="162"/>
       <c r="W22" s="162"/>
     </row>
-    <row r="23" spans="1:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>185</v>
       </c>
@@ -10721,7 +10721,7 @@
       <c r="V23" s="162"/>
       <c r="W23" s="162"/>
     </row>
-    <row r="24" spans="1:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>186</v>
       </c>
@@ -10755,7 +10755,7 @@
       <c r="V24" s="162"/>
       <c r="W24" s="162"/>
     </row>
-    <row r="25" spans="1:42" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>187</v>
       </c>
@@ -10786,17 +10786,17 @@
       <c r="V25" s="162"/>
       <c r="W25" s="162"/>
     </row>
-    <row r="26" spans="1:42" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C27" s="71"/>
     </row>
-    <row r="28" spans="1:42" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:42" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="70"/>
       <c r="H28" s="107"/>
       <c r="I28" s="107"/>
       <c r="J28" s="107"/>
     </row>
-    <row r="29" spans="1:42" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:42" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="101" t="s">
         <v>170</v>
       </c>
@@ -10835,7 +10835,7 @@
       <c r="W29" s="214"/>
       <c r="X29" s="214"/>
     </row>
-    <row r="30" spans="1:42" ht="21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:42" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="100" t="s">
         <v>169</v>
       </c>
@@ -10905,7 +10905,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C31" s="109" t="s">
         <v>129</v>
       </c>
@@ -10944,7 +10944,7 @@
       <c r="T31" s="109"/>
       <c r="U31" s="109"/>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C32" s="110" t="s">
         <v>130</v>
       </c>
@@ -10983,7 +10983,7 @@
       <c r="T32" s="110"/>
       <c r="U32" s="110"/>
     </row>
-    <row r="33" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C33" s="110" t="s">
         <v>131</v>
       </c>
@@ -11025,7 +11025,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C34" s="110" t="s">
         <v>132</v>
       </c>
@@ -11064,7 +11064,7 @@
       <c r="T34" s="110"/>
       <c r="U34" s="110"/>
     </row>
-    <row r="35" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C35" s="110" t="s">
         <v>133</v>
       </c>
@@ -11103,7 +11103,7 @@
       <c r="T35" s="110"/>
       <c r="U35" s="110"/>
     </row>
-    <row r="36" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C36" s="110" t="s">
         <v>134</v>
       </c>
@@ -11142,7 +11142,7 @@
       <c r="T36" s="110"/>
       <c r="U36" s="110"/>
     </row>
-    <row r="37" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C37" s="111" t="s">
         <v>135</v>
       </c>
@@ -11211,7 +11211,7 @@
         <v>7.4868583865827593E-2</v>
       </c>
     </row>
-    <row r="38" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C38" s="109" t="s">
         <v>136</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>0.11688125511605342</v>
       </c>
     </row>
-    <row r="39" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C39" s="111" t="s">
         <v>137</v>
       </c>
@@ -11351,7 +11351,7 @@
         <v>1.6202273564329378E-2</v>
       </c>
     </row>
-    <row r="40" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C40" s="110" t="s">
         <v>138</v>
       </c>
@@ -11420,7 +11420,7 @@
         <v>0.13130393418469363</v>
       </c>
     </row>
-    <row r="41" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C41" s="109" t="s">
         <v>139</v>
       </c>
@@ -11489,7 +11489,7 @@
         <v>8.1230839111318301E-2</v>
       </c>
     </row>
-    <row r="42" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C42" s="111" t="s">
         <v>140</v>
       </c>
@@ -11564,7 +11564,7 @@
         <v>7.3172573402951982E-2</v>
       </c>
     </row>
-    <row r="43" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C43" s="110" t="s">
         <v>141</v>
       </c>
@@ -11633,7 +11633,7 @@
         <v>9.234697345696842E-2</v>
       </c>
     </row>
-    <row r="44" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C44" s="109" t="s">
         <v>142</v>
       </c>
@@ -11702,7 +11702,7 @@
         <v>7.1161885518135765E-2</v>
       </c>
     </row>
-    <row r="45" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C45" s="110" t="s">
         <v>143</v>
       </c>
@@ -11776,7 +11776,7 @@
         <v>6.7752568250727771E-2</v>
       </c>
     </row>
-    <row r="46" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C46" s="111" t="s">
         <v>144</v>
       </c>
@@ -11851,7 +11851,7 @@
         <v>3.6794477883422452E-2</v>
       </c>
     </row>
-    <row r="47" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C47" s="110" t="s">
         <v>145</v>
       </c>
@@ -11920,7 +11920,7 @@
         <v>4.8388466845630869E-2</v>
       </c>
     </row>
-    <row r="48" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C48" s="109" t="s">
         <v>146</v>
       </c>
@@ -11989,7 +11989,7 @@
         <v>4.0577241203268805E-2</v>
       </c>
     </row>
-    <row r="49" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C49" s="110" t="s">
         <v>147</v>
       </c>
@@ -12063,7 +12063,7 @@
         <v>3.9320180267811942E-2</v>
       </c>
     </row>
-    <row r="50" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C50" s="110" t="s">
         <v>148</v>
       </c>
@@ -12136,7 +12136,7 @@
         <v>2.7905517746048429E-2</v>
       </c>
     </row>
-    <row r="51" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C51" s="111" t="s">
         <v>149</v>
       </c>
@@ -12207,7 +12207,7 @@
         <v>1.4338900983817031E-2</v>
       </c>
     </row>
-    <row r="52" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C52" s="110" t="s">
         <v>150</v>
       </c>
@@ -12258,7 +12258,7 @@
       <c r="W52" s="117"/>
       <c r="X52" s="117"/>
     </row>
-    <row r="53" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C53" s="109" t="s">
         <v>151</v>
       </c>
@@ -12327,7 +12327,7 @@
         <v>5.1020288697720552E-2</v>
       </c>
     </row>
-    <row r="54" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C54" s="110" t="s">
         <v>152</v>
       </c>
@@ -12400,7 +12400,7 @@
         <v>4.9525094922424191E-2</v>
       </c>
     </row>
-    <row r="55" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C55" s="110" t="s">
         <v>153</v>
       </c>
@@ -12478,7 +12478,7 @@
         <v>3.5948082171290856E-2</v>
       </c>
     </row>
-    <row r="56" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C56" s="110" t="s">
         <v>154</v>
       </c>
@@ -12553,7 +12553,7 @@
         <v>1.9811457157685314E-2</v>
       </c>
     </row>
-    <row r="57" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C57" s="112" t="s">
         <v>176</v>
       </c>
@@ -12621,7 +12621,7 @@
         <v>2.7562493385017966E-3</v>
       </c>
     </row>
-    <row r="59" spans="3:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:24" x14ac:dyDescent="0.2">
       <c r="S59" s="120">
         <f>SUM(S37,S39,S42,S46,S51,S57)</f>
         <v>9608.4735804205193</v>
@@ -12647,7 +12647,7 @@
         <v>0.21813305903885022</v>
       </c>
     </row>
-    <row r="60" spans="3:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
         <v>175</v>
       </c>

</xml_diff>